<commit_message>
changes due to null records
</commit_message>
<xml_diff>
--- a/MIRACLEECOMMERCEFRAMEWORK.xlsx
+++ b/MIRACLEECOMMERCEFRAMEWORK.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miracle\Desktop\all\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miracle\eclipse-workspace\Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8340" activeTab="3"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="19560" windowHeight="8340" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SCENARIOS" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="196">
   <si>
     <t>HEADER</t>
   </si>
@@ -600,13 +600,29 @@
   </si>
   <si>
     <t xml:space="preserve">LOGIN </t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Output as expected</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>User is unable to perform operation on that element</t>
+  </si>
+  <si>
+    <t>Invalid Keywords are mentioned</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="175" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -702,8 +718,976 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="215">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -756,6 +1740,955 @@
       <patternFill patternType="solid">
         <fgColor indexed="60"/>
         <bgColor indexed="25"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -801,7 +2734,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -867,11 +2800,499 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="53" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="54" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="55" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="58" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="59" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="60" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="61" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="62" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="63" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="64" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="65" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="66" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="67" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="68" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="69" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="70" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="71" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="72" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="73" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="74" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="75" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="76" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="77" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="78" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="79" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="80" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="81" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="82" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="83" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="84" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="85" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="88" fillId="86" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="87" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="88" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="90" fillId="90" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="92" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="93" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="93" fillId="95" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="96" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="98" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="99" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="101" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="102" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="104" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="105" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="107" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="108" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="110" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="111" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="113" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="106" fillId="114" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="116" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="117" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="116" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="110" fillId="119" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="120" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="112" fillId="122" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="113" fillId="123" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="114" fillId="125" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="115" fillId="126" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="116" fillId="128" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="117" fillId="129" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="118" fillId="131" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="132" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="120" fillId="134" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="121" fillId="135" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="122" fillId="137" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="123" fillId="138" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="124" fillId="140" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="125" fillId="141" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="126" fillId="143" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="127" fillId="144" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="128" fillId="146" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="129" fillId="147" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="130" fillId="149" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="131" fillId="150" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="132" fillId="152" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="133" fillId="153" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="134" fillId="155" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="135" fillId="156" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="136" fillId="158" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="137" fillId="159" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="138" fillId="161" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="139" fillId="162" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="140" fillId="164" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="141" fillId="165" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="142" fillId="167" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="143" fillId="168" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="144" fillId="170" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="145" fillId="172" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="146" fillId="173" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="147" fillId="175" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="148" fillId="176" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="149" fillId="178" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="150" fillId="179" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="151" fillId="178" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="152" fillId="181" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="153" fillId="182" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="154" fillId="184" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="155" fillId="185" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="156" fillId="187" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="157" fillId="188" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="158" fillId="190" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="159" fillId="191" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="160" fillId="193" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="161" fillId="194" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="162" fillId="196" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="163" fillId="198" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="164" fillId="199" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="165" fillId="201" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="166" fillId="202" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="167" fillId="204" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="168" fillId="205" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="169" fillId="207" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="170" fillId="208" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="171" fillId="210" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="172" fillId="211" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="173" fillId="213" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment wrapText="true" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="174" fillId="214" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment wrapText="true" horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1225,198 +3646,198 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="14" customWidth="1"/>
-    <col min="3" max="256" width="8.7109375" style="14"/>
-    <col min="257" max="257" width="36.28515625" style="14" customWidth="1"/>
-    <col min="258" max="258" width="17.28515625" style="14" customWidth="1"/>
-    <col min="259" max="512" width="8.7109375" style="14"/>
-    <col min="513" max="513" width="36.28515625" style="14" customWidth="1"/>
-    <col min="514" max="514" width="17.28515625" style="14" customWidth="1"/>
-    <col min="515" max="768" width="8.7109375" style="14"/>
-    <col min="769" max="769" width="36.28515625" style="14" customWidth="1"/>
-    <col min="770" max="770" width="17.28515625" style="14" customWidth="1"/>
-    <col min="771" max="1024" width="8.7109375" style="14"/>
-    <col min="1025" max="1025" width="36.28515625" style="14" customWidth="1"/>
-    <col min="1026" max="1026" width="17.28515625" style="14" customWidth="1"/>
-    <col min="1027" max="1280" width="8.7109375" style="14"/>
-    <col min="1281" max="1281" width="36.28515625" style="14" customWidth="1"/>
-    <col min="1282" max="1282" width="17.28515625" style="14" customWidth="1"/>
-    <col min="1283" max="1536" width="8.7109375" style="14"/>
-    <col min="1537" max="1537" width="36.28515625" style="14" customWidth="1"/>
-    <col min="1538" max="1538" width="17.28515625" style="14" customWidth="1"/>
-    <col min="1539" max="1792" width="8.7109375" style="14"/>
-    <col min="1793" max="1793" width="36.28515625" style="14" customWidth="1"/>
-    <col min="1794" max="1794" width="17.28515625" style="14" customWidth="1"/>
-    <col min="1795" max="2048" width="8.7109375" style="14"/>
-    <col min="2049" max="2049" width="36.28515625" style="14" customWidth="1"/>
-    <col min="2050" max="2050" width="17.28515625" style="14" customWidth="1"/>
-    <col min="2051" max="2304" width="8.7109375" style="14"/>
-    <col min="2305" max="2305" width="36.28515625" style="14" customWidth="1"/>
-    <col min="2306" max="2306" width="17.28515625" style="14" customWidth="1"/>
-    <col min="2307" max="2560" width="8.7109375" style="14"/>
-    <col min="2561" max="2561" width="36.28515625" style="14" customWidth="1"/>
-    <col min="2562" max="2562" width="17.28515625" style="14" customWidth="1"/>
-    <col min="2563" max="2816" width="8.7109375" style="14"/>
-    <col min="2817" max="2817" width="36.28515625" style="14" customWidth="1"/>
-    <col min="2818" max="2818" width="17.28515625" style="14" customWidth="1"/>
-    <col min="2819" max="3072" width="8.7109375" style="14"/>
-    <col min="3073" max="3073" width="36.28515625" style="14" customWidth="1"/>
-    <col min="3074" max="3074" width="17.28515625" style="14" customWidth="1"/>
-    <col min="3075" max="3328" width="8.7109375" style="14"/>
-    <col min="3329" max="3329" width="36.28515625" style="14" customWidth="1"/>
-    <col min="3330" max="3330" width="17.28515625" style="14" customWidth="1"/>
-    <col min="3331" max="3584" width="8.7109375" style="14"/>
-    <col min="3585" max="3585" width="36.28515625" style="14" customWidth="1"/>
-    <col min="3586" max="3586" width="17.28515625" style="14" customWidth="1"/>
-    <col min="3587" max="3840" width="8.7109375" style="14"/>
-    <col min="3841" max="3841" width="36.28515625" style="14" customWidth="1"/>
-    <col min="3842" max="3842" width="17.28515625" style="14" customWidth="1"/>
-    <col min="3843" max="4096" width="8.7109375" style="14"/>
-    <col min="4097" max="4097" width="36.28515625" style="14" customWidth="1"/>
-    <col min="4098" max="4098" width="17.28515625" style="14" customWidth="1"/>
-    <col min="4099" max="4352" width="8.7109375" style="14"/>
-    <col min="4353" max="4353" width="36.28515625" style="14" customWidth="1"/>
-    <col min="4354" max="4354" width="17.28515625" style="14" customWidth="1"/>
-    <col min="4355" max="4608" width="8.7109375" style="14"/>
-    <col min="4609" max="4609" width="36.28515625" style="14" customWidth="1"/>
-    <col min="4610" max="4610" width="17.28515625" style="14" customWidth="1"/>
-    <col min="4611" max="4864" width="8.7109375" style="14"/>
-    <col min="4865" max="4865" width="36.28515625" style="14" customWidth="1"/>
-    <col min="4866" max="4866" width="17.28515625" style="14" customWidth="1"/>
-    <col min="4867" max="5120" width="8.7109375" style="14"/>
-    <col min="5121" max="5121" width="36.28515625" style="14" customWidth="1"/>
-    <col min="5122" max="5122" width="17.28515625" style="14" customWidth="1"/>
-    <col min="5123" max="5376" width="8.7109375" style="14"/>
-    <col min="5377" max="5377" width="36.28515625" style="14" customWidth="1"/>
-    <col min="5378" max="5378" width="17.28515625" style="14" customWidth="1"/>
-    <col min="5379" max="5632" width="8.7109375" style="14"/>
-    <col min="5633" max="5633" width="36.28515625" style="14" customWidth="1"/>
-    <col min="5634" max="5634" width="17.28515625" style="14" customWidth="1"/>
-    <col min="5635" max="5888" width="8.7109375" style="14"/>
-    <col min="5889" max="5889" width="36.28515625" style="14" customWidth="1"/>
-    <col min="5890" max="5890" width="17.28515625" style="14" customWidth="1"/>
-    <col min="5891" max="6144" width="8.7109375" style="14"/>
-    <col min="6145" max="6145" width="36.28515625" style="14" customWidth="1"/>
-    <col min="6146" max="6146" width="17.28515625" style="14" customWidth="1"/>
-    <col min="6147" max="6400" width="8.7109375" style="14"/>
-    <col min="6401" max="6401" width="36.28515625" style="14" customWidth="1"/>
-    <col min="6402" max="6402" width="17.28515625" style="14" customWidth="1"/>
-    <col min="6403" max="6656" width="8.7109375" style="14"/>
-    <col min="6657" max="6657" width="36.28515625" style="14" customWidth="1"/>
-    <col min="6658" max="6658" width="17.28515625" style="14" customWidth="1"/>
-    <col min="6659" max="6912" width="8.7109375" style="14"/>
-    <col min="6913" max="6913" width="36.28515625" style="14" customWidth="1"/>
-    <col min="6914" max="6914" width="17.28515625" style="14" customWidth="1"/>
-    <col min="6915" max="7168" width="8.7109375" style="14"/>
-    <col min="7169" max="7169" width="36.28515625" style="14" customWidth="1"/>
-    <col min="7170" max="7170" width="17.28515625" style="14" customWidth="1"/>
-    <col min="7171" max="7424" width="8.7109375" style="14"/>
-    <col min="7425" max="7425" width="36.28515625" style="14" customWidth="1"/>
-    <col min="7426" max="7426" width="17.28515625" style="14" customWidth="1"/>
-    <col min="7427" max="7680" width="8.7109375" style="14"/>
-    <col min="7681" max="7681" width="36.28515625" style="14" customWidth="1"/>
-    <col min="7682" max="7682" width="17.28515625" style="14" customWidth="1"/>
-    <col min="7683" max="7936" width="8.7109375" style="14"/>
-    <col min="7937" max="7937" width="36.28515625" style="14" customWidth="1"/>
-    <col min="7938" max="7938" width="17.28515625" style="14" customWidth="1"/>
-    <col min="7939" max="8192" width="8.7109375" style="14"/>
-    <col min="8193" max="8193" width="36.28515625" style="14" customWidth="1"/>
-    <col min="8194" max="8194" width="17.28515625" style="14" customWidth="1"/>
-    <col min="8195" max="8448" width="8.7109375" style="14"/>
-    <col min="8449" max="8449" width="36.28515625" style="14" customWidth="1"/>
-    <col min="8450" max="8450" width="17.28515625" style="14" customWidth="1"/>
-    <col min="8451" max="8704" width="8.7109375" style="14"/>
-    <col min="8705" max="8705" width="36.28515625" style="14" customWidth="1"/>
-    <col min="8706" max="8706" width="17.28515625" style="14" customWidth="1"/>
-    <col min="8707" max="8960" width="8.7109375" style="14"/>
-    <col min="8961" max="8961" width="36.28515625" style="14" customWidth="1"/>
-    <col min="8962" max="8962" width="17.28515625" style="14" customWidth="1"/>
-    <col min="8963" max="9216" width="8.7109375" style="14"/>
-    <col min="9217" max="9217" width="36.28515625" style="14" customWidth="1"/>
-    <col min="9218" max="9218" width="17.28515625" style="14" customWidth="1"/>
-    <col min="9219" max="9472" width="8.7109375" style="14"/>
-    <col min="9473" max="9473" width="36.28515625" style="14" customWidth="1"/>
-    <col min="9474" max="9474" width="17.28515625" style="14" customWidth="1"/>
-    <col min="9475" max="9728" width="8.7109375" style="14"/>
-    <col min="9729" max="9729" width="36.28515625" style="14" customWidth="1"/>
-    <col min="9730" max="9730" width="17.28515625" style="14" customWidth="1"/>
-    <col min="9731" max="9984" width="8.7109375" style="14"/>
-    <col min="9985" max="9985" width="36.28515625" style="14" customWidth="1"/>
-    <col min="9986" max="9986" width="17.28515625" style="14" customWidth="1"/>
-    <col min="9987" max="10240" width="8.7109375" style="14"/>
-    <col min="10241" max="10241" width="36.28515625" style="14" customWidth="1"/>
-    <col min="10242" max="10242" width="17.28515625" style="14" customWidth="1"/>
-    <col min="10243" max="10496" width="8.7109375" style="14"/>
-    <col min="10497" max="10497" width="36.28515625" style="14" customWidth="1"/>
-    <col min="10498" max="10498" width="17.28515625" style="14" customWidth="1"/>
-    <col min="10499" max="10752" width="8.7109375" style="14"/>
-    <col min="10753" max="10753" width="36.28515625" style="14" customWidth="1"/>
-    <col min="10754" max="10754" width="17.28515625" style="14" customWidth="1"/>
-    <col min="10755" max="11008" width="8.7109375" style="14"/>
-    <col min="11009" max="11009" width="36.28515625" style="14" customWidth="1"/>
-    <col min="11010" max="11010" width="17.28515625" style="14" customWidth="1"/>
-    <col min="11011" max="11264" width="8.7109375" style="14"/>
-    <col min="11265" max="11265" width="36.28515625" style="14" customWidth="1"/>
-    <col min="11266" max="11266" width="17.28515625" style="14" customWidth="1"/>
-    <col min="11267" max="11520" width="8.7109375" style="14"/>
-    <col min="11521" max="11521" width="36.28515625" style="14" customWidth="1"/>
-    <col min="11522" max="11522" width="17.28515625" style="14" customWidth="1"/>
-    <col min="11523" max="11776" width="8.7109375" style="14"/>
-    <col min="11777" max="11777" width="36.28515625" style="14" customWidth="1"/>
-    <col min="11778" max="11778" width="17.28515625" style="14" customWidth="1"/>
-    <col min="11779" max="12032" width="8.7109375" style="14"/>
-    <col min="12033" max="12033" width="36.28515625" style="14" customWidth="1"/>
-    <col min="12034" max="12034" width="17.28515625" style="14" customWidth="1"/>
-    <col min="12035" max="12288" width="8.7109375" style="14"/>
-    <col min="12289" max="12289" width="36.28515625" style="14" customWidth="1"/>
-    <col min="12290" max="12290" width="17.28515625" style="14" customWidth="1"/>
-    <col min="12291" max="12544" width="8.7109375" style="14"/>
-    <col min="12545" max="12545" width="36.28515625" style="14" customWidth="1"/>
-    <col min="12546" max="12546" width="17.28515625" style="14" customWidth="1"/>
-    <col min="12547" max="12800" width="8.7109375" style="14"/>
-    <col min="12801" max="12801" width="36.28515625" style="14" customWidth="1"/>
-    <col min="12802" max="12802" width="17.28515625" style="14" customWidth="1"/>
-    <col min="12803" max="13056" width="8.7109375" style="14"/>
-    <col min="13057" max="13057" width="36.28515625" style="14" customWidth="1"/>
-    <col min="13058" max="13058" width="17.28515625" style="14" customWidth="1"/>
-    <col min="13059" max="13312" width="8.7109375" style="14"/>
-    <col min="13313" max="13313" width="36.28515625" style="14" customWidth="1"/>
-    <col min="13314" max="13314" width="17.28515625" style="14" customWidth="1"/>
-    <col min="13315" max="13568" width="8.7109375" style="14"/>
-    <col min="13569" max="13569" width="36.28515625" style="14" customWidth="1"/>
-    <col min="13570" max="13570" width="17.28515625" style="14" customWidth="1"/>
-    <col min="13571" max="13824" width="8.7109375" style="14"/>
-    <col min="13825" max="13825" width="36.28515625" style="14" customWidth="1"/>
-    <col min="13826" max="13826" width="17.28515625" style="14" customWidth="1"/>
-    <col min="13827" max="14080" width="8.7109375" style="14"/>
-    <col min="14081" max="14081" width="36.28515625" style="14" customWidth="1"/>
-    <col min="14082" max="14082" width="17.28515625" style="14" customWidth="1"/>
-    <col min="14083" max="14336" width="8.7109375" style="14"/>
-    <col min="14337" max="14337" width="36.28515625" style="14" customWidth="1"/>
-    <col min="14338" max="14338" width="17.28515625" style="14" customWidth="1"/>
-    <col min="14339" max="14592" width="8.7109375" style="14"/>
-    <col min="14593" max="14593" width="36.28515625" style="14" customWidth="1"/>
-    <col min="14594" max="14594" width="17.28515625" style="14" customWidth="1"/>
-    <col min="14595" max="14848" width="8.7109375" style="14"/>
-    <col min="14849" max="14849" width="36.28515625" style="14" customWidth="1"/>
-    <col min="14850" max="14850" width="17.28515625" style="14" customWidth="1"/>
-    <col min="14851" max="15104" width="8.7109375" style="14"/>
-    <col min="15105" max="15105" width="36.28515625" style="14" customWidth="1"/>
-    <col min="15106" max="15106" width="17.28515625" style="14" customWidth="1"/>
-    <col min="15107" max="15360" width="8.7109375" style="14"/>
-    <col min="15361" max="15361" width="36.28515625" style="14" customWidth="1"/>
-    <col min="15362" max="15362" width="17.28515625" style="14" customWidth="1"/>
-    <col min="15363" max="15616" width="8.7109375" style="14"/>
-    <col min="15617" max="15617" width="36.28515625" style="14" customWidth="1"/>
-    <col min="15618" max="15618" width="17.28515625" style="14" customWidth="1"/>
-    <col min="15619" max="15872" width="8.7109375" style="14"/>
-    <col min="15873" max="15873" width="36.28515625" style="14" customWidth="1"/>
-    <col min="15874" max="15874" width="17.28515625" style="14" customWidth="1"/>
-    <col min="15875" max="16128" width="8.7109375" style="14"/>
-    <col min="16129" max="16129" width="36.28515625" style="14" customWidth="1"/>
-    <col min="16130" max="16130" width="17.28515625" style="14" customWidth="1"/>
-    <col min="16131" max="16384" width="8.7109375" style="14"/>
+    <col min="1" max="1" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="3" max="256" style="14" width="8.7109375" collapsed="true"/>
+    <col min="257" max="257" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="258" max="258" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="259" max="512" style="14" width="8.7109375" collapsed="true"/>
+    <col min="513" max="513" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="514" max="514" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="515" max="768" style="14" width="8.7109375" collapsed="true"/>
+    <col min="769" max="769" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="770" max="770" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="771" max="1024" style="14" width="8.7109375" collapsed="true"/>
+    <col min="1025" max="1025" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="1026" max="1026" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="1027" max="1280" style="14" width="8.7109375" collapsed="true"/>
+    <col min="1281" max="1281" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="1282" max="1282" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="1283" max="1536" style="14" width="8.7109375" collapsed="true"/>
+    <col min="1537" max="1537" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="1538" max="1538" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="1539" max="1792" style="14" width="8.7109375" collapsed="true"/>
+    <col min="1793" max="1793" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="1794" max="1794" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="1795" max="2048" style="14" width="8.7109375" collapsed="true"/>
+    <col min="2049" max="2049" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="2050" max="2050" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="2051" max="2304" style="14" width="8.7109375" collapsed="true"/>
+    <col min="2305" max="2305" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="2306" max="2306" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="2307" max="2560" style="14" width="8.7109375" collapsed="true"/>
+    <col min="2561" max="2561" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="2562" max="2562" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="2563" max="2816" style="14" width="8.7109375" collapsed="true"/>
+    <col min="2817" max="2817" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="2818" max="2818" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="2819" max="3072" style="14" width="8.7109375" collapsed="true"/>
+    <col min="3073" max="3073" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="3074" max="3074" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="3075" max="3328" style="14" width="8.7109375" collapsed="true"/>
+    <col min="3329" max="3329" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="3330" max="3330" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="3331" max="3584" style="14" width="8.7109375" collapsed="true"/>
+    <col min="3585" max="3585" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="3586" max="3586" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="3587" max="3840" style="14" width="8.7109375" collapsed="true"/>
+    <col min="3841" max="3841" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="3842" max="3842" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="3843" max="4096" style="14" width="8.7109375" collapsed="true"/>
+    <col min="4097" max="4097" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="4098" max="4098" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="4099" max="4352" style="14" width="8.7109375" collapsed="true"/>
+    <col min="4353" max="4353" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="4354" max="4354" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="4355" max="4608" style="14" width="8.7109375" collapsed="true"/>
+    <col min="4609" max="4609" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="4610" max="4610" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="4611" max="4864" style="14" width="8.7109375" collapsed="true"/>
+    <col min="4865" max="4865" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="4866" max="4866" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="4867" max="5120" style="14" width="8.7109375" collapsed="true"/>
+    <col min="5121" max="5121" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="5122" max="5122" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="5123" max="5376" style="14" width="8.7109375" collapsed="true"/>
+    <col min="5377" max="5377" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="5378" max="5378" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="5379" max="5632" style="14" width="8.7109375" collapsed="true"/>
+    <col min="5633" max="5633" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="5634" max="5634" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="5635" max="5888" style="14" width="8.7109375" collapsed="true"/>
+    <col min="5889" max="5889" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="5890" max="5890" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="5891" max="6144" style="14" width="8.7109375" collapsed="true"/>
+    <col min="6145" max="6145" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="6146" max="6146" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="6147" max="6400" style="14" width="8.7109375" collapsed="true"/>
+    <col min="6401" max="6401" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="6402" max="6402" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="6403" max="6656" style="14" width="8.7109375" collapsed="true"/>
+    <col min="6657" max="6657" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="6658" max="6658" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="6659" max="6912" style="14" width="8.7109375" collapsed="true"/>
+    <col min="6913" max="6913" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="6914" max="6914" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="6915" max="7168" style="14" width="8.7109375" collapsed="true"/>
+    <col min="7169" max="7169" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="7170" max="7170" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="7171" max="7424" style="14" width="8.7109375" collapsed="true"/>
+    <col min="7425" max="7425" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="7426" max="7426" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="7427" max="7680" style="14" width="8.7109375" collapsed="true"/>
+    <col min="7681" max="7681" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="7682" max="7682" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="7683" max="7936" style="14" width="8.7109375" collapsed="true"/>
+    <col min="7937" max="7937" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="7938" max="7938" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="7939" max="8192" style="14" width="8.7109375" collapsed="true"/>
+    <col min="8193" max="8193" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="8194" max="8194" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="8195" max="8448" style="14" width="8.7109375" collapsed="true"/>
+    <col min="8449" max="8449" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="8450" max="8450" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="8451" max="8704" style="14" width="8.7109375" collapsed="true"/>
+    <col min="8705" max="8705" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="8706" max="8706" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="8707" max="8960" style="14" width="8.7109375" collapsed="true"/>
+    <col min="8961" max="8961" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="8962" max="8962" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="8963" max="9216" style="14" width="8.7109375" collapsed="true"/>
+    <col min="9217" max="9217" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="9218" max="9218" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="9219" max="9472" style="14" width="8.7109375" collapsed="true"/>
+    <col min="9473" max="9473" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="9474" max="9474" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="9475" max="9728" style="14" width="8.7109375" collapsed="true"/>
+    <col min="9729" max="9729" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="9730" max="9730" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="9731" max="9984" style="14" width="8.7109375" collapsed="true"/>
+    <col min="9985" max="9985" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="9986" max="9986" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="9987" max="10240" style="14" width="8.7109375" collapsed="true"/>
+    <col min="10241" max="10241" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="10242" max="10242" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="10243" max="10496" style="14" width="8.7109375" collapsed="true"/>
+    <col min="10497" max="10497" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="10498" max="10498" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="10499" max="10752" style="14" width="8.7109375" collapsed="true"/>
+    <col min="10753" max="10753" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="10754" max="10754" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="10755" max="11008" style="14" width="8.7109375" collapsed="true"/>
+    <col min="11009" max="11009" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="11010" max="11010" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="11011" max="11264" style="14" width="8.7109375" collapsed="true"/>
+    <col min="11265" max="11265" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="11266" max="11266" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="11267" max="11520" style="14" width="8.7109375" collapsed="true"/>
+    <col min="11521" max="11521" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="11522" max="11522" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="11523" max="11776" style="14" width="8.7109375" collapsed="true"/>
+    <col min="11777" max="11777" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="11778" max="11778" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="11779" max="12032" style="14" width="8.7109375" collapsed="true"/>
+    <col min="12033" max="12033" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="12034" max="12034" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="12035" max="12288" style="14" width="8.7109375" collapsed="true"/>
+    <col min="12289" max="12289" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="12290" max="12290" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="12291" max="12544" style="14" width="8.7109375" collapsed="true"/>
+    <col min="12545" max="12545" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="12546" max="12546" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="12547" max="12800" style="14" width="8.7109375" collapsed="true"/>
+    <col min="12801" max="12801" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="12802" max="12802" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="12803" max="13056" style="14" width="8.7109375" collapsed="true"/>
+    <col min="13057" max="13057" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="13058" max="13058" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="13059" max="13312" style="14" width="8.7109375" collapsed="true"/>
+    <col min="13313" max="13313" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="13314" max="13314" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="13315" max="13568" style="14" width="8.7109375" collapsed="true"/>
+    <col min="13569" max="13569" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="13570" max="13570" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="13571" max="13824" style="14" width="8.7109375" collapsed="true"/>
+    <col min="13825" max="13825" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="13826" max="13826" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="13827" max="14080" style="14" width="8.7109375" collapsed="true"/>
+    <col min="14081" max="14081" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="14082" max="14082" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="14083" max="14336" style="14" width="8.7109375" collapsed="true"/>
+    <col min="14337" max="14337" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="14338" max="14338" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="14339" max="14592" style="14" width="8.7109375" collapsed="true"/>
+    <col min="14593" max="14593" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="14594" max="14594" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="14595" max="14848" style="14" width="8.7109375" collapsed="true"/>
+    <col min="14849" max="14849" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="14850" max="14850" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="14851" max="15104" style="14" width="8.7109375" collapsed="true"/>
+    <col min="15105" max="15105" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="15106" max="15106" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="15107" max="15360" style="14" width="8.7109375" collapsed="true"/>
+    <col min="15361" max="15361" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="15362" max="15362" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="15363" max="15616" style="14" width="8.7109375" collapsed="true"/>
+    <col min="15617" max="15617" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="15618" max="15618" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="15619" max="15872" style="14" width="8.7109375" collapsed="true"/>
+    <col min="15873" max="15873" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="15874" max="15874" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="15875" max="16128" style="14" width="8.7109375" collapsed="true"/>
+    <col min="16129" max="16129" customWidth="true" style="14" width="36.28515625" collapsed="true"/>
+    <col min="16130" max="16130" customWidth="true" style="14" width="17.28515625" collapsed="true"/>
+    <col min="16131" max="16384" style="14" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1443,7 +3864,9 @@
       <c r="C2" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" t="s" s="137">
+        <v>193</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -1455,7 +3878,9 @@
       <c r="C3" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" t="s" s="179">
+        <v>193</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
@@ -1467,7 +3892,9 @@
       <c r="C4" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D4" s="27"/>
+      <c r="D4" t="s" s="190">
+        <v>191</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
@@ -1477,7 +3904,7 @@
         <v>172</v>
       </c>
       <c r="C5" s="7"/>
-      <c r="D5" s="27"/>
+      <c r="D5" s="117"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1487,7 +3914,7 @@
         <v>174</v>
       </c>
       <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="D6" s="117"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1497,7 +3924,7 @@
         <v>176</v>
       </c>
       <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="117"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1507,7 +3934,7 @@
         <v>178</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="117"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -1517,7 +3944,7 @@
         <v>180</v>
       </c>
       <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="D9" s="117"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1527,7 +3954,7 @@
         <v>182</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="D10" s="117"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -1537,7 +3964,7 @@
         <v>184</v>
       </c>
       <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="D11" s="117"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -1547,13 +3974,21 @@
         <v>186</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="D12" s="117"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" location="APAC-02_HomePage_Footer!A1" display="APAC-02_HomePage_Footer"/>
     <hyperlink ref="A4" location="'APAC-29 Login'!A1" display="APAC-29 Login"/>
     <hyperlink ref="A5" location="APAC-031_Forgot Password!A1" display="APAC-031_Forgot Password"/>
+    <hyperlink ref="D2" location="'SUMMARY'!A1" tooltip="This is Invalid Keyword. Please click on LINK. Find correct KEYWORD in SUMMARY sheet. Thank you!!!" display="Invalid Keywords are mentioned"/>
+    <hyperlink ref="D2" location="'SUMMARY'!A1" tooltip="This is Invalid Keyword. Please click on LINK. Find correct KEYWORD in SUMMARY sheet. Thank you!!!" display="Invalid Keywords are mentioned"/>
+    <hyperlink ref="D2" location="'SUMMARY'!A1" tooltip="This is Invalid Keyword. Please click on LINK. Find correct KEYWORD in SUMMARY sheet. Thank you!!!" display="Invalid Keywords are mentioned"/>
+    <hyperlink ref="D2" location="'SUMMARY'!A1" tooltip="This is Invalid Keyword. Please click on LINK. Find correct KEYWORD in SUMMARY sheet. Thank you!!!" display="Invalid Keywords are mentioned"/>
+    <hyperlink ref="D2" location="'SUMMARY'!A1" tooltip="This is Invalid Keyword. Please click on LINK. Find correct KEYWORD in SUMMARY sheet. Thank you!!!" display="Invalid Keywords are mentioned"/>
+    <hyperlink ref="D2" location="'SUMMARY'!A1" tooltip="This is Invalid Keyword. Please click on LINK. Find correct KEYWORD in SUMMARY sheet. Thank you!!!" display="Invalid Keywords are mentioned"/>
+    <hyperlink ref="D2" location="'SUMMARY'!A1" tooltip="This is Invalid Keyword. Please click on LINK. Find correct KEYWORD in SUMMARY sheet. Thank you!!!" display="Invalid Keywords are mentioned"/>
+    <hyperlink ref="D2" location="'SUMMARY'!A1" tooltip="This is Invalid Keyword. Please click on LINK. Find correct KEYWORD in SUMMARY sheet. Thank you!!!" display="Invalid Keywords are mentioned"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1569,26 +4004,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="40.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1637,8 +4072,12 @@
       <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
+      <c r="H3" t="s" s="174">
+        <v>192</v>
+      </c>
+      <c r="I3" t="s" s="173">
+        <v>191</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1683,8 +4122,12 @@
       <c r="G5" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
+      <c r="H5" t="s" s="176">
+        <v>192</v>
+      </c>
+      <c r="I5" t="s" s="175">
+        <v>191</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -1729,8 +4172,12 @@
       <c r="G7" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="10"/>
+      <c r="H7" t="s" s="178">
+        <v>194</v>
+      </c>
+      <c r="I7" t="s" s="177">
+        <v>193</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1775,8 +4222,12 @@
       <c r="G9" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="13"/>
+      <c r="H9" t="s" s="181">
+        <v>192</v>
+      </c>
+      <c r="I9" t="s" s="180">
+        <v>191</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1821,8 +4272,12 @@
       <c r="G11" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="H11" t="s" s="183">
+        <v>192</v>
+      </c>
+      <c r="I11" t="s" s="182">
+        <v>191</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1867,8 +4322,12 @@
       <c r="G13" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="H13" t="s" s="185">
+        <v>192</v>
+      </c>
+      <c r="I13" t="s" s="184">
+        <v>191</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -1913,8 +4372,12 @@
       <c r="G15" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+      <c r="H15" t="s" s="187">
+        <v>192</v>
+      </c>
+      <c r="I15" t="s" s="186">
+        <v>191</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -1959,8 +4422,12 @@
       <c r="G17" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="H17" t="s" s="189">
+        <v>192</v>
+      </c>
+      <c r="I17" t="s" s="188">
+        <v>191</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -2006,23 +4473,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="31.7109375" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" customWidth="1"/>
-    <col min="7" max="7" width="34.28515625" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="116" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2071,8 +4538,12 @@
       <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
+      <c r="H3" t="s" s="192">
+        <v>192</v>
+      </c>
+      <c r="I3" t="s" s="191">
+        <v>191</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -2094,8 +4565,12 @@
       <c r="G4" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
+      <c r="H4" t="s" s="194">
+        <v>192</v>
+      </c>
+      <c r="I4" t="s" s="193">
+        <v>191</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -2119,8 +4594,12 @@
       <c r="G5" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
+      <c r="H5" t="s" s="196">
+        <v>192</v>
+      </c>
+      <c r="I5" t="s" s="195">
+        <v>191</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -2165,8 +4644,12 @@
       <c r="G7" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="10"/>
+      <c r="H7" t="s" s="198">
+        <v>192</v>
+      </c>
+      <c r="I7" t="s" s="197">
+        <v>191</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -2211,8 +4694,12 @@
       <c r="G9" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="13"/>
+      <c r="H9" t="s" s="200">
+        <v>192</v>
+      </c>
+      <c r="I9" t="s" s="199">
+        <v>191</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -2255,8 +4742,12 @@
       <c r="G11" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="H11" t="s" s="202">
+        <v>192</v>
+      </c>
+      <c r="I11" t="s" s="201">
+        <v>191</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -2297,33 +4788,33 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
-      <selection sqref="A1:I36"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="C36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="33.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="38.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="116" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -2372,8 +4863,12 @@
       <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
+      <c r="H3" t="s" s="120">
+        <v>192</v>
+      </c>
+      <c r="I3" t="s" s="119">
+        <v>191</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -2437,8 +4932,12 @@
       <c r="G6" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10"/>
+      <c r="H6" t="s" s="122">
+        <v>192</v>
+      </c>
+      <c r="I6" t="s" s="121">
+        <v>191</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -2460,8 +4959,12 @@
       <c r="G7" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="10"/>
+      <c r="H7" t="s" s="124">
+        <v>192</v>
+      </c>
+      <c r="I7" t="s" s="123">
+        <v>191</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -2483,8 +4986,12 @@
       <c r="G8" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="10"/>
+      <c r="H8" t="s" s="126">
+        <v>192</v>
+      </c>
+      <c r="I8" t="s" s="125">
+        <v>191</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -2527,8 +5034,12 @@
       <c r="G10" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="H10" t="s" s="128">
+        <v>192</v>
+      </c>
+      <c r="I10" t="s" s="127">
+        <v>191</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -2550,8 +5061,12 @@
       <c r="G11" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="H11" t="s" s="130">
+        <v>192</v>
+      </c>
+      <c r="I11" t="s" s="129">
+        <v>191</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -2573,8 +5088,12 @@
       <c r="G12" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
+      <c r="H12" t="s" s="132">
+        <v>192</v>
+      </c>
+      <c r="I12" t="s" s="131">
+        <v>191</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -2596,8 +5115,12 @@
       <c r="G13" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="H13" t="s" s="134">
+        <v>192</v>
+      </c>
+      <c r="I13" t="s" s="133">
+        <v>191</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -2640,8 +5163,12 @@
       <c r="G15" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+      <c r="H15" t="s" s="136">
+        <v>194</v>
+      </c>
+      <c r="I15" t="s" s="135">
+        <v>193</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -2663,8 +5190,12 @@
       <c r="G16" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
+      <c r="H16" t="s" s="139">
+        <v>192</v>
+      </c>
+      <c r="I16" t="s" s="138">
+        <v>191</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -2686,8 +5217,12 @@
       <c r="G17" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="H17" t="s" s="141">
+        <v>192</v>
+      </c>
+      <c r="I17" t="s" s="140">
+        <v>191</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -2709,8 +5244,12 @@
       <c r="G18" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="H18" t="s" s="143">
+        <v>192</v>
+      </c>
+      <c r="I18" t="s" s="142">
+        <v>191</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -2753,8 +5292,12 @@
       <c r="G20" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="H20" t="s" s="145">
+        <v>192</v>
+      </c>
+      <c r="I20" t="s" s="144">
+        <v>191</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -2776,8 +5319,12 @@
       <c r="G21" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
+      <c r="H21" t="s" s="147">
+        <v>192</v>
+      </c>
+      <c r="I21" t="s" s="146">
+        <v>191</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
@@ -2799,8 +5346,12 @@
       <c r="G22" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="H22" t="s" s="149">
+        <v>192</v>
+      </c>
+      <c r="I22" t="s" s="148">
+        <v>191</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -2822,8 +5373,12 @@
       <c r="G23" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
+      <c r="H23" t="s" s="151">
+        <v>192</v>
+      </c>
+      <c r="I23" t="s" s="150">
+        <v>191</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -2866,8 +5421,12 @@
       <c r="G25" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
+      <c r="H25" t="s" s="153">
+        <v>192</v>
+      </c>
+      <c r="I25" t="s" s="152">
+        <v>191</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -2889,8 +5448,12 @@
       <c r="G26" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
+      <c r="H26" t="s" s="155">
+        <v>192</v>
+      </c>
+      <c r="I26" t="s" s="154">
+        <v>191</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -2912,8 +5475,12 @@
       <c r="G27" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
+      <c r="H27" t="s" s="157">
+        <v>192</v>
+      </c>
+      <c r="I27" t="s" s="156">
+        <v>191</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -2935,8 +5502,12 @@
       <c r="G28" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
+      <c r="H28" t="s" s="159">
+        <v>192</v>
+      </c>
+      <c r="I28" t="s" s="158">
+        <v>191</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -2960,8 +5531,12 @@
       <c r="G29" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
+      <c r="H29" t="s" s="161">
+        <v>192</v>
+      </c>
+      <c r="I29" t="s" s="160">
+        <v>191</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
@@ -2985,10 +5560,14 @@
       <c r="G30" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" t="s" s="163">
+        <v>192</v>
+      </c>
+      <c r="I30" t="s" s="162">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>63</v>
       </c>
@@ -3008,10 +5587,14 @@
       <c r="G31" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" t="s" s="165">
+        <v>192</v>
+      </c>
+      <c r="I31" t="s" s="164">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>64</v>
       </c>
@@ -3033,8 +5616,12 @@
       <c r="G32" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
+      <c r="H32" t="s" s="167">
+        <v>192</v>
+      </c>
+      <c r="I32" t="s" s="166">
+        <v>191</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
@@ -3057,7 +5644,7 @@
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>66</v>
       </c>
@@ -3079,10 +5666,14 @@
       <c r="G34" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H34" t="s" s="169">
+        <v>192</v>
+      </c>
+      <c r="I34" t="s" s="168">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>67</v>
       </c>
@@ -3104,10 +5695,13 @@
       <c r="G35" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-    </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+      <c r="H35" t="s" s="171">
+        <v>192</v>
+      </c>
+      <c r="I35" t="s" s="170">
+        <v>191</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>

</xml_diff>